<commit_message>
Updated test data for XLSX file
</commit_message>
<xml_diff>
--- a/testData/LoginData.xlsx
+++ b/testData/LoginData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Module\automation-assignment\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Java Module\Test Automation Framework\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C867415-502D-4F67-AECF-47E670FFFE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -350,20 +349,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -371,7 +370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Fixed for relative path
</commit_message>
<xml_diff>
--- a/testData/LoginData.xlsx
+++ b/testData/LoginData.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Java Module\Test Automation Framework\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13890"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="6135"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>emailAddress</t>
   </si>
@@ -33,6 +29,9 @@
   </si>
   <si>
     <t>timotoj174@asaption.com</t>
+  </si>
+  <si>
+    <t>kalpeshk354@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -350,10 +349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,8 +377,19 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>123456</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>